<commit_message>
within-motif, across-motif aggregation best_combo: sasa: mean,sum flex: max, sum
</commit_message>
<xml_diff>
--- a/results/metric_df/AMA_metrics.xlsx
+++ b/results/metric_df/AMA_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SASA</t>
+          <t>monosaccharides</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>sum_SASA</t>
+          <t>motifs</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>max_SASA</t>
+          <t>sasa</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -466,32 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>theta</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>conformation</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>monosaccharides</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>motifs</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>class</t>
+          <t>has_multi_node_motifs</t>
         </is>
       </c>
     </row>
@@ -504,43 +479,24 @@
       <c r="B2" t="n">
         <v>2.210633079814709</v>
       </c>
-      <c r="C2" t="n">
-        <v>2.190741739754425</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>4.38148347950885</v>
       </c>
-      <c r="E2" t="n">
-        <v>2.708633284112756</v>
-      </c>
       <c r="F2" t="n">
-        <v>12.77328732873287</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.3945</v>
-      </c>
-      <c r="H2" t="n">
-        <v>45.555</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>['B2,5', '4C1']</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2)', 'Man(a1-6)']</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>3.557542575354189</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -552,43 +508,24 @@
       <c r="B3" t="n">
         <v>1.811659352547796</v>
       </c>
-      <c r="C3" t="n">
-        <v>2.40522749318555</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>4.8104549863711</v>
       </c>
-      <c r="E3" t="n">
-        <v>3.126238794575282</v>
-      </c>
       <c r="F3" t="n">
-        <v>17.31664285714286</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="H3" t="n">
-        <v>9.845000000000001</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2)', 'Man(a1-3)']</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>4.822931845266804</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -600,43 +537,24 @@
       <c r="B4" t="n">
         <v>4.349188472075032</v>
       </c>
-      <c r="C4" t="n">
-        <v>2.297728771163197</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>9.190915084652787</v>
       </c>
-      <c r="E4" t="n">
-        <v>3.138514975631664</v>
-      </c>
       <c r="F4" t="n">
-        <v>10.06704003733707</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.43475</v>
-      </c>
-      <c r="H4" t="n">
-        <v>9.065</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>6.308581799857853</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -648,235 +566,314 @@
       <c r="B5" t="n">
         <v>-0.1125181812871801</v>
       </c>
-      <c r="C5" t="n">
-        <v>2.390937431966916</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9.563749727867664</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
       </c>
       <c r="E5" t="n">
-        <v>3.183609109940719</v>
+        <v>9.563749727867666</v>
       </c>
       <c r="F5" t="n">
-        <v>12.36463853614639</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.43775</v>
-      </c>
-      <c r="H5" t="n">
-        <v>6.54</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>6.887456124510353</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Man(a1-2)Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-4)][GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7290354871251824</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2.112871867249531</v>
-      </c>
-      <c r="D6" t="n">
-        <v>6.338615601748595</v>
+        <v>-0.2304548244600497</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
       </c>
       <c r="E6" t="n">
-        <v>2.251887232513918</v>
+        <v>8.702690750097064</v>
       </c>
       <c r="F6" t="n">
-        <v>36.56924074074075</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.4133333333333333</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6.386666666666667</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)', 'Man(a1-2)', 'Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>7.677022565287091</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Man(a1-2)Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-6)[Man(a1-3)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)[GlcNAc(b1-6)]Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.298700425902069</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2.483961017275276</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.967922034550551</v>
+        <v>-0.2154724433322029</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
       </c>
       <c r="E7" t="n">
-        <v>2.505235247011588</v>
+        <v>8.635859486927</v>
       </c>
       <c r="F7" t="n">
-        <v>36.76748333333335</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.4635</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)', 'Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>6.932052642066758</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Man(a1-2)Man(a1-3)[Man(a1-3)[Man(a1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)[GlcNAc(b1-6)]Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.049472015187181</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2.414822869487025</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2.414822869487025</v>
+        <v>-0.2143122440556122</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'GlcNAc(b1-2)', 'Man(a1-6)']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2/4)Man(a1-?)']</t>
+        </is>
       </c>
       <c r="E8" t="n">
-        <v>2.414822869487025</v>
+        <v>8.640812173985104</v>
       </c>
       <c r="F8" t="n">
-        <v>17.55984285714286</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.452</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>['4C1']</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>['Man(a1-2)']</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+        <v>9.849110063284527</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>Man(a1-2)Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.7290354871251824</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)', 'Man(a1-2)', 'Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>6.338615601748595</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11.45818660281608</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Man(a1-2)Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-6)[Man(a1-3)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.298700425902069</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)', 'Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>4.967922034550551</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8.378401210032491</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Man(a1-2)Man(a1-3)[Man(a1-2)Man(a1-6)]Man(a1-6)[Man(a1-2)Man(a1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.479130577311217</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)', 'Man(a1-2)', 'Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>6.338615601748595</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11.45818660281608</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Man(a1-2)Man(a1-3)[Man(a1-3)[Man(a1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.049472015187181</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2.414822869487025</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2.445333255766194</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
           <t>Man(a1-2)Man(a1-3)[Man(a1-6)]Man(a1-6)[Man(a1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B13" t="n">
         <v>2.086895142638032</v>
       </c>
-      <c r="C9" t="n">
-        <v>2.134344346283708</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)', 'Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>4.268688692567416</v>
       </c>
-      <c r="E9" t="n">
-        <v>2.33250225642029</v>
-      </c>
-      <c r="F9" t="n">
-        <v>20.3436</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.4535</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.28</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="F13" t="n">
+        <v>5.099384296778321</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Man(a1-2)Man(a1-6)[Man(a1-3)]Man(a1-6)[Man(a1-2)Man(a1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.907438974643126</v>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>['Man(a1-2)', 'Man(a1-2)']</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>['Man(a1-2)']</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+      <c r="E14" t="n">
+        <v>4.967922034550551</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8.378401210032491</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Man(a1-3)[Man(a1-6)]Man(a1-6)[Man(a1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>8.555836977700899</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['Man(a1-2)']</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2.414822869487025</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2.445333255766194</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>